<commit_message>
Changing count to 150
</commit_message>
<xml_diff>
--- a/twitterSentimentals.xlsx
+++ b/twitterSentimentals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="179">
   <si>
     <t>texts</t>
   </si>
@@ -25,23 +25,300 @@
     <t>created_at</t>
   </si>
   <si>
-    <t xml:space="preserve"> One year ago in Davos for the World Economic Forum  - having a chat over coffee with . Feels like ages ago, o…</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> We updated this years' #excibitions and we really hope that we will be able to attend some of them and meet some of you p…</t>
+    <t xml:space="preserve">IWH medium-term projection for 🇩🇪 until 2025: #GDP grows more slowly than before (by an average of ½%) due to… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Today the #Steam (#Steamkey or #Steamkeys) #givaway Saturday for #final_m00n - Defender of the Cubes.
+20 #free final m00n -…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sweden on Bidens travel ban!
+#whocouldhaveknown #shocker #gofigure #FHM #sweden #Corona #COVID19 #bidentravelban #Biden #Har…</t>
   </si>
   <si>
     <t xml:space="preserve"> while #corona is supposed to hit all of us equally, the extreme rich have only become richer and the poor have become poorer.…</t>
   </si>
   <si>
-    <t xml:space="preserve"> People in #Germany soon could face a major shortage of fruits and vegetables imported from #Spain, #Portugal, #Italy,…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Factinsect in Steiermark heute: don't miss out on this great reporting on our start-up!
-(1:29) 2:55 - 3:55 Min)… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Mexico`s president #AMLO has #coronavirus: After an event in San Luis Potosí, President #LópezObrador informed tha… </t>
+    <t xml:space="preserve">Today the #Steam (#Steamkey or #Steamkeys) #givaway Saturday for #final_m00n - Defender of the Cubes.
+20 #free fina… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check out Sam Spencer's video! #TikTok #mondaythoughts #corona #justforfun </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockdown and Motherhood
+Miki Shaw, an artist, illustrator and graphic designer based in London, reflects on parenth… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Is AI the future of dating in 2021?  
+#AI #5G #MachineLearning #DataScience #Python #100DaysOfCode #…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This error message is from an official german website that is supposed to help 80+ year olds get an vaccination date. Throwing 504…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moved into a coworking space with lots of desks unavailable due to Corona. Still a good energy while everybody is taking pr…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy monday everyone! Prepare for your online meetings and smiiiiiiiiile 😁
+#StayAtHome #JitsiMeet #Corona… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have questions about the #COVID19 #vaccine? Read #JHAH frequently asked questions to know about the benefits… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moved into a coworking space with lots of desks unavailable due to Corona. Still a good energy while everybody is t… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parents appreciate #learnwhilesittingathome. #Corona can force us to #StayHome but can't stop learning. We  trying our be…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pain of #corona #isolation is morphing into a comforting block builder
+Too many faces and too many eyes used to… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reopening of #Schools:  gears up to aware #teachers, #students on #Corona SOPs  
+RK Onli… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NSAIDs might exacerbate or suppress #COVID19 depending on timing
+#Research #…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSAIDs might exacerbate or suppress #COVID19 depending on timing
+… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait! Wasn't this fake news not long ago? The #colchicine and #Hydroxychloroquine were no-good harmful and toxic?… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Challenges in #vaccination against the #coronavirus will be discussed by experts Gagandeep Kang, ,… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heart disease risk associated with eating fried foods
+#Research #drugdiscove…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heart disease risk associated with eating fried foods
+#Research… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #COVID19 : Harrowing reality of a coronavirus ward 
+#Research #vaccina…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#COVID19 : Harrowing reality of a coronavirus ward 
+#Research… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Corona #Birdflu #Viruses all are bcoz of Animal Killings which #Humans have to Keep Facing Untill Entire 🌎 World d… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Relief Th. and Acer Th. sign option agreement for exclusivity to negotiate a collaboration and license agreement for t…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In Western countries health institutions ignore the elderly, the poor, people with Down syndrome &amp;amp; so on, because these pe…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> About praying in sacred sites during #Ramadan, I believe the National Committee on Combating #Corona’s opinions are valid,…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #diabetes treatment may protect against #COVID19 mortality
+#Research #…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#diabetes treatment may protect against #COVID19 mortality
+… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In an #interview with  , our CEO Elisabeth Stadler talked about what has changed at VIG as a result of…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> “Tesla Has Better AI Hardware &amp;amp; Software Than Waymo”  
+#Tesla #ElonMusk #AI #5G #MachineLearning #Da…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New on BRAVE NEW EUROPE
+Real and Fictitious Capital: The COVID stock market europhoria
+Michael Roberts – Covid an… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Patents valid only inside Your People's republic of #Corona. Coz outside you'll be sued for IP inf… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium vitamins &amp;amp; supplements for every stage of life! 
+#StayHealthy #Corona #Covid_19… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Targomo supports Leipzig Health Department to contain pandemic - A good example of how #locationtechnology is being… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sven Dietrich co-founded V-MD Group along with Sylvio. He works as a freelance cameraman. Sven is also an avid land… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#TransferNews #Fenerbache swoop on #Iheanacho after #Ozil #transfer coup #Nigeria #football #PremierLeague #lcfc… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no support for entrepreneurs for livelihood.Government has closed their shop and expect that they live wit… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   You definitely have a soft spot for People's Republic of #Corona or Xhina.… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Netherlands #CoronaRiots #CivilWar #Corona #avondklokrellen   
+Mayor of Eindhoven, Jorritsma: If the sit… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Who gets priority when Covid-19 shots are in short supply? Network theorists have a counterintuitive answer: Start… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ok, that may be true. It worked to a certain extend. The underlying problems still are aro… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Tesla Has Better AI Hardware &amp;amp; Software Than Waymo”  
+#Tesla #ElonMusk #AI #5G… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM Modi interacts with recipients of Rashtriya Bal Puraskar, 2021  
+#PMModi #RashtriyaBalPuraskar #SmritiZubinIrani… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask you cleaner for a touch clean today and help keep the virus at bay #virus #corona #antibacteria #choresnpawsintl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saudi Press|
+Ministry of Health Calls for Adherence to Precautionary Measures
+-
+… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check out a blog post by  telling how he created #live maps of Germany visualizing various #corona-relate… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Also in the EU the perpetrators of climate change are determining our future strategy
+Positive Money …</t>
+  </si>
+  <si>
+    <t>#Wuhan #SARSCoV2 #COVID19 #Corona #vaccination                 ✨ONLY PEOPLE THAT BELIEVE IN COVID 19 CATCH COVID 19 ✨</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Google today announced that Google Search and Maps will show vaccination locations in the United States.… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24 Jan
+#DelhiFightsCorona 
+🔻 185 NEW #Corona cases 
+TOTAL- 6,33,924 cases
+🔹 315 Recovered today,
+TOTAL Recovered- 6,21,3…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#RepublicDay2021 :
+No Beating Retreat Ceremony at #Wagah 
+due to #Corona #Pandemic ?
+.
+.
+.
+How about #Delhi ?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is AI the future of dating in 2021?  
+#AI #5G #MachineLearning #DataScience #Python… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Seems legit, to me. Of course this will also not work for #Corona, just as it failed to wo… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look the part in 2021
+▶️   ◀️
+#BEARD #romeos #mentalhealth #mondaythoughts #selfcare… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">History of #Corona virus! #COVID19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In order that our life returns as it was in the past, I #ChoosetoVaccinate, and I invite you all to take the initia… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Kapitalismus und #Corona als Brandbeschleuniger: "We stand to witness the greatest rise in inequality since record… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prime Minister  interacted with  #RashtriyaBalPuraskar awardees today via video conferencing; said that this ye…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#coronabadhairchallenge
+These Times are weird. Only our Haircuts are more weird. Show us, what you got.
+#badhair… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you ever wondered if you're a twat? 
+Well, I've devised this test, backed by the scientists, for you to find… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y’all hear me out!! Maybe if we all held hands and made a big group circle, ofc while wearing mask and gloves, and… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trapped by Stupids in the Mental Zombie Apocalypse : Foamy The Squirrel  via … </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #China selling Corona Vaccine reminds me of man owning puncture repair shop on highway and use to throw nails  on highway f…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #Corona is affecting rich and poor without discrimination, says #PMImranKhan 
+#Live: 
+#PublicN…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden on Bidens travel ban!
+#whocouldhaveknown #shocker #gofigure #FHM #sweden #Corona #COVID19 #bidentravelban… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagine waking up to a new day with no lockdown &amp;amp; no coronavirus, I'm even wondering what it would feel like😫What w… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Africa -related news content from APO Group -updates on #Corona #virus  in Africa via … </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Get your orders in for our famous #ParkingBuddies for delivery during #lockdown
+Customise them to suit your #school colo…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dirty tricks dept of global disease hub &amp;amp; #corona nation #China at work. #Sinovac being rejected while Indian #vaccine…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prime Minister  interacted with  #RashtriyaBalPuraskar awardees today via video conferencing; said tha… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This tweet is simply tragic perfection.
+It tells the never ending story of the delusions &amp;amp; denials that callously leave…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The same happend to $XVS and look at it now!
+$Vidt will explode! 28 Million MCAP 49 Million Coins!… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This error message is from an official german website that is supposed to help 80+ year olds get an vaccination dat… </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #Bihar continues to report more recoveries than fresh #Corona cases. 267 patients recovered during the past 24 hours, whil…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get your orders in for our famous #ParkingBuddies for delivery during #lockdown
+Customise them to suit your #school… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents are feeling the strain
+of teaching at home yet again.
+It looks nearly certain
+school’s gone for a burton
+th… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">So it hasn’t been approved.. #COVID19 #Covid19UK #CoronaVaccine #Corona </t>
+  </si>
+  <si>
+    <t>neutral</t>
   </si>
   <si>
     <t>positive</t>
@@ -50,34 +327,286 @@
     <t>negative</t>
   </si>
   <si>
-    <t>neutral</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:37:55 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:37:37 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:37:25 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:35:00 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:33:53 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:32:57 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:31:49 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:31:29 +0000 2021</t>
-  </si>
-  <si>
-    <t>Mon Jan 25 08:31:05 +0000 2021</t>
+    <t>Mon Jan 25 10:41:10 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:41:03 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:40:35 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:40:20 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:40:02 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:38:04 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:37:15 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:36:16 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:36:03 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:35:45 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:35:30 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:31:35 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:30:53 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:29:17 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:28:41 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:28:14 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:26:42 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:26:32 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:25:29 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:24:18 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:22:44 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:22:36 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:21:30 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:21:24 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:20:19 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:20:13 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:18:36 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:18:30 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:17:20 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:16:32 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:16:04 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:15:57 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:15:47 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:15:41 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:13:49 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:09:29 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:09:20 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:08:47 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:07:53 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:07:24 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:06:54 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:06:24 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:05:36 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:05:32 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:04:54 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:04:30 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:02:53 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:02:43 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:02:13 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:02:08 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:01:21 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:00:32 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 10:00:00 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:58:50 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:57:42 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:57:22 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:56:21 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:56:04 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:56:02 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:59 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:57 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:56 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:54 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:29 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:26 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:24 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:19 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:55:00 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:54:21 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:52:25 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:52:00 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:49:43 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:47:40 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:45:37 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:44:25 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:44:14 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:44:05 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:42:31 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:42:24 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:41:10 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:40:26 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:40:22 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:39:57 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:39:51 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:39:42 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:39:36 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:39:33 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:38:44 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:37:57 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:36:46 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:35:45 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:35:41 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:35:07 +0000 2021</t>
+  </si>
+  <si>
+    <t>Mon Jan 25 09:35:03 +0000 2021</t>
   </si>
 </sst>
 </file>
@@ -435,7 +964,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,10 +986,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -468,10 +997,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -479,10 +1008,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -490,76 +1019,1066 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>60</v>
+      </c>
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>65</v>
+      </c>
+      <c r="B81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+      <c r="C86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>83</v>
+      </c>
+      <c r="C87" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>71</v>
+      </c>
+      <c r="B88" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>72</v>
+      </c>
+      <c r="B89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" t="s">
+        <v>84</v>
+      </c>
+      <c r="C90" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>62</v>
+      </c>
+      <c r="B91" t="s">
+        <v>83</v>
+      </c>
+      <c r="C91" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>74</v>
+      </c>
+      <c r="B92" t="s">
+        <v>83</v>
+      </c>
+      <c r="C92" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>83</v>
+      </c>
+      <c r="C93" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>75</v>
+      </c>
+      <c r="B94" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" t="s">
+        <v>82</v>
+      </c>
+      <c r="C95" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>77</v>
+      </c>
+      <c r="B96" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>78</v>
+      </c>
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>80</v>
+      </c>
+      <c r="B99" t="s">
+        <v>83</v>
+      </c>
+      <c r="C99" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>81</v>
+      </c>
+      <c r="B100" t="s">
+        <v>83</v>
+      </c>
+      <c r="C100" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>73</v>
+      </c>
+      <c r="B101" t="s">
+        <v>84</v>
+      </c>
+      <c r="C101" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>